<commit_message>
change the summary statistics
</commit_message>
<xml_diff>
--- a/summary_statistics.xlsx
+++ b/summary_statistics.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6940" activeTab="1" xr2:uid="{7B30B581-41F3-4625-9AEB-EDD9A381FEDF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6940" activeTab="2" xr2:uid="{7B30B581-41F3-4625-9AEB-EDD9A381FEDF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="66">
   <si>
     <t>African Amer/Black</t>
   </si>
@@ -202,6 +203,27 @@
   </si>
   <si>
     <t>visit ICU during hospitalization</t>
+  </si>
+  <si>
+    <t>02sat</t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>Respiration Rate</t>
+  </si>
+  <si>
+    <t>Heart Rate</t>
+  </si>
+  <si>
+    <t>mean_arterial_pressure</t>
+  </si>
+  <si>
+    <t>Length of stay (hours)</t>
+  </si>
+  <si>
+    <t>Length of stay (days)</t>
   </si>
 </sst>
 </file>
@@ -254,7 +276,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -270,12 +292,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -287,11 +303,20 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -607,10 +632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B5EFC5A-2BC7-489C-88B9-EDFF87E125F6}">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView zoomScale="66" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -627,73 +652,87 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="2"/>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="10" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
+      <c r="A3" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="9">
+        <v>129.9</v>
+      </c>
+      <c r="C3" s="9">
+        <v>91</v>
+      </c>
+      <c r="D3" s="9">
+        <v>139.30000000000001</v>
+      </c>
+      <c r="E3" s="9">
+        <v>51</v>
+      </c>
+      <c r="F3" s="9">
+        <v>161</v>
+      </c>
+      <c r="G3" s="9">
+        <v>1</v>
+      </c>
+      <c r="H3" s="9">
+        <v>1861</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="2">
-        <v>1.31</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1.33</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0.89</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0.75</v>
-      </c>
-      <c r="F4" s="10">
-        <v>1.9</v>
-      </c>
-      <c r="G4" s="2">
-        <v>-3.18</v>
-      </c>
-      <c r="H4" s="2">
-        <v>4.3499999999999996</v>
+        <v>65</v>
+      </c>
+      <c r="B4" s="3">
+        <v>5.41</v>
+      </c>
+      <c r="C4" s="3">
+        <v>3.79</v>
+      </c>
+      <c r="D4" s="3">
+        <v>5.81</v>
+      </c>
+      <c r="E4" s="3">
+        <v>2.13</v>
+      </c>
+      <c r="F4" s="8">
+        <v>6.71</v>
+      </c>
+      <c r="G4" s="8">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="H4" s="3">
+        <v>77.540000000000006</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -703,22 +742,22 @@
       <c r="B5" s="2">
         <v>1.73</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="8">
         <v>1</v>
       </c>
       <c r="D5" s="2">
         <v>1.58</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="8">
         <v>0</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="8">
         <v>3</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="8">
         <v>0</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5" s="8">
         <v>4</v>
       </c>
     </row>
@@ -729,7 +768,7 @@
       <c r="B6" s="2">
         <v>65</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="3">
         <v>67</v>
       </c>
       <c r="D6" s="2">
@@ -770,503 +809,555 @@
       <c r="G7" s="2">
         <v>3.1</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="9">
         <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="2">
-        <v>1.6699999999999999E-4</v>
-      </c>
-      <c r="C8" s="2">
-        <v>1.5899999999999999E-4</v>
-      </c>
-      <c r="D8" s="2">
-        <v>5.3499999999999999E-5</v>
-      </c>
-      <c r="E8" s="2">
-        <v>1.2999999999999999E-4</v>
-      </c>
-      <c r="F8" s="2">
-        <v>1.9799999999999999E-4</v>
-      </c>
-      <c r="G8" s="2">
-        <v>1.7E-5</v>
-      </c>
-      <c r="H8" s="2">
-        <v>7.0799999999999997E-4</v>
+        <v>59</v>
+      </c>
+      <c r="B8" s="3">
+        <v>97.9</v>
+      </c>
+      <c r="C8" s="3">
+        <v>97.6</v>
+      </c>
+      <c r="D8" s="3">
+        <v>5.27</v>
+      </c>
+      <c r="E8" s="3">
+        <v>96.53</v>
+      </c>
+      <c r="F8" s="3">
+        <v>98.6</v>
+      </c>
+      <c r="G8" s="3">
+        <v>80</v>
+      </c>
+      <c r="H8" s="9">
+        <v>236.53</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>21</v>
+        <v>60</v>
       </c>
       <c r="B9" s="2">
-        <v>3.1199999999999999E-3</v>
+        <v>36.75</v>
       </c>
       <c r="C9" s="2">
-        <v>3.1700000000000001E-3</v>
-      </c>
-      <c r="D9" s="2">
-        <v>5.4699999999999996E-4</v>
+        <v>36.729999999999997</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.79</v>
       </c>
       <c r="E9" s="2">
-        <v>2.9299999999999999E-3</v>
+        <v>36.61</v>
       </c>
       <c r="F9" s="2">
-        <v>3.4199999999999999E-3</v>
-      </c>
-      <c r="G9" s="2">
-        <v>2.1800000000000001E-4</v>
+        <v>36.869999999999997</v>
+      </c>
+      <c r="G9" s="8">
+        <v>30</v>
       </c>
       <c r="H9" s="2">
-        <v>6.94E-3</v>
+        <v>52.28</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="11">
-        <v>140</v>
-      </c>
-      <c r="C10" s="11">
+        <v>62</v>
+      </c>
+      <c r="B10" s="8">
+        <v>80.2</v>
+      </c>
+      <c r="C10" s="2">
+        <v>79.349999999999994</v>
+      </c>
+      <c r="D10" s="2">
+        <v>13.31</v>
+      </c>
+      <c r="E10" s="2">
+        <v>71.12</v>
+      </c>
+      <c r="F10" s="2">
+        <v>87.71</v>
+      </c>
+      <c r="G10" s="2">
+        <v>37.58</v>
+      </c>
+      <c r="H10" s="2">
+        <v>242.58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="9">
+        <v>18.22</v>
+      </c>
+      <c r="C11" s="9">
+        <v>17.75</v>
+      </c>
+      <c r="D11" s="2">
+        <v>2.78</v>
+      </c>
+      <c r="E11" s="9">
+        <v>17.09</v>
+      </c>
+      <c r="F11" s="9">
+        <v>18.48</v>
+      </c>
+      <c r="G11" s="9">
+        <v>12</v>
+      </c>
+      <c r="H11" s="9">
+        <v>67.72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" s="9">
+        <v>140.24</v>
+      </c>
+      <c r="C12" s="9">
         <v>139</v>
       </c>
-      <c r="D10" s="2">
-        <v>16.399999999999999</v>
-      </c>
-      <c r="E10" s="11">
-        <v>129</v>
-      </c>
-      <c r="F10" s="11">
-        <v>150</v>
-      </c>
-      <c r="G10" s="11">
+      <c r="D12" s="9">
+        <v>16.41</v>
+      </c>
+      <c r="E12" s="9">
+        <v>128.85</v>
+      </c>
+      <c r="F12" s="9">
+        <v>149.69999999999999</v>
+      </c>
+      <c r="G12" s="9">
         <v>90.9</v>
       </c>
-      <c r="H10" s="11">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
+      <c r="H12" s="9">
+        <v>252.3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B13" s="2"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="2">
-        <v>1.33</v>
-      </c>
-      <c r="C13" s="2">
-        <v>1.34</v>
-      </c>
-      <c r="D13" s="2">
-        <v>0.8</v>
-      </c>
-      <c r="E13" s="2">
-        <v>0.75</v>
-      </c>
-      <c r="F13" s="10">
-        <v>1.9</v>
-      </c>
-      <c r="G13" s="2">
-        <v>-1.23</v>
-      </c>
-      <c r="H13" s="2">
-        <v>3.92</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="2">
-        <v>1.74</v>
-      </c>
-      <c r="C14" s="10">
-        <v>1</v>
-      </c>
-      <c r="D14" s="2">
-        <v>1.58</v>
-      </c>
-      <c r="E14" s="10">
-        <v>0</v>
-      </c>
-      <c r="F14" s="10">
-        <v>3</v>
-      </c>
-      <c r="G14" s="10">
-        <v>0</v>
-      </c>
-      <c r="H14" s="10">
-        <v>4</v>
-      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B15" s="2">
-        <v>65.2</v>
-      </c>
-      <c r="C15" s="11">
-        <v>67</v>
+        <v>1.33</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1.34</v>
       </c>
       <c r="D15" s="2">
-        <v>18.5</v>
-      </c>
-      <c r="E15" s="11">
-        <v>53</v>
-      </c>
-      <c r="F15" s="11">
-        <v>80</v>
-      </c>
-      <c r="G15" s="11">
-        <v>18</v>
-      </c>
-      <c r="H15" s="11">
-        <v>101</v>
+        <v>0.8</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="F15" s="8">
+        <v>1.9</v>
+      </c>
+      <c r="G15" s="2">
+        <v>-1.23</v>
+      </c>
+      <c r="H15" s="2">
+        <v>3.92</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B16" s="2">
-        <v>28.4</v>
-      </c>
-      <c r="C16" s="2">
-        <v>27.1</v>
-      </c>
-      <c r="D16" s="11">
-        <v>8</v>
-      </c>
-      <c r="E16" s="2">
-        <v>23.3</v>
-      </c>
-      <c r="F16" s="2">
-        <v>31.7</v>
-      </c>
-      <c r="G16" s="2">
-        <v>3.1</v>
-      </c>
-      <c r="H16" s="11">
-        <v>123</v>
+        <v>1.74</v>
+      </c>
+      <c r="C16" s="8">
+        <v>1</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1.58</v>
+      </c>
+      <c r="E16" s="8">
+        <v>0</v>
+      </c>
+      <c r="F16" s="8">
+        <v>3</v>
+      </c>
+      <c r="G16" s="8">
+        <v>0</v>
+      </c>
+      <c r="H16" s="8">
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" s="2">
-        <v>1.6799999999999999E-4</v>
-      </c>
-      <c r="C17" s="2">
-        <v>1.5899999999999999E-4</v>
+        <v>65.2</v>
+      </c>
+      <c r="C17" s="9">
+        <v>67</v>
       </c>
       <c r="D17" s="2">
-        <v>5.38E-5</v>
-      </c>
-      <c r="E17" s="2">
-        <v>1.2999999999999999E-4</v>
-      </c>
-      <c r="F17" s="2">
-        <v>1.9799999999999999E-4</v>
-      </c>
-      <c r="G17" s="2">
-        <v>1.7E-5</v>
-      </c>
-      <c r="H17" s="2">
-        <v>7.0799999999999997E-4</v>
+        <v>18.5</v>
+      </c>
+      <c r="E17" s="9">
+        <v>53</v>
+      </c>
+      <c r="F17" s="9">
+        <v>80</v>
+      </c>
+      <c r="G17" s="9">
+        <v>18</v>
+      </c>
+      <c r="H17" s="9">
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B18" s="2">
-        <v>3.13E-3</v>
+        <v>28.4</v>
       </c>
       <c r="C18" s="2">
-        <v>3.1800000000000001E-3</v>
-      </c>
-      <c r="D18" s="2">
-        <v>5.4100000000000003E-4</v>
+        <v>27.1</v>
+      </c>
+      <c r="D18" s="9">
+        <v>8</v>
       </c>
       <c r="E18" s="2">
-        <v>2.9299999999999999E-3</v>
+        <v>23.3</v>
       </c>
       <c r="F18" s="2">
-        <v>3.4199999999999999E-3</v>
+        <v>31.7</v>
       </c>
       <c r="G18" s="2">
-        <v>2.1800000000000001E-4</v>
-      </c>
-      <c r="H18" s="2">
-        <v>5.5100000000000001E-3</v>
+        <v>3.1</v>
+      </c>
+      <c r="H18" s="9">
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1.6799999999999999E-4</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1.5899999999999999E-4</v>
+      </c>
+      <c r="D19" s="2">
+        <v>5.38E-5</v>
+      </c>
+      <c r="E19" s="2">
+        <v>1.2999999999999999E-4</v>
+      </c>
+      <c r="F19" s="2">
+        <v>1.9799999999999999E-4</v>
+      </c>
+      <c r="G19" s="2">
+        <v>1.7E-5</v>
+      </c>
+      <c r="H19" s="2">
+        <v>7.0799999999999997E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="2">
+        <v>3.13E-3</v>
+      </c>
+      <c r="C20" s="2">
+        <v>3.1800000000000001E-3</v>
+      </c>
+      <c r="D20" s="2">
+        <v>5.4100000000000003E-4</v>
+      </c>
+      <c r="E20" s="2">
+        <v>2.9299999999999999E-3</v>
+      </c>
+      <c r="F20" s="2">
+        <v>3.4199999999999999E-3</v>
+      </c>
+      <c r="G20" s="2">
+        <v>2.1800000000000001E-4</v>
+      </c>
+      <c r="H20" s="2">
+        <v>5.5100000000000001E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="11">
+      <c r="B21" s="9">
         <v>140</v>
       </c>
-      <c r="C19" s="11">
+      <c r="C21" s="9">
         <v>139</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D21" s="2">
         <v>16.399999999999999</v>
       </c>
-      <c r="E19" s="11">
+      <c r="E21" s="9">
         <v>129</v>
       </c>
-      <c r="F19" s="11">
+      <c r="F21" s="9">
         <v>150</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G21" s="2">
         <v>90.9</v>
       </c>
-      <c r="H19" s="11">
+      <c r="H21" s="9">
         <v>252</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="C22" s="10">
-        <v>-0.9</v>
-      </c>
-      <c r="D22" s="2">
-        <v>3.05</v>
-      </c>
-      <c r="E22" s="10">
-        <v>-3</v>
-      </c>
-      <c r="F22" s="2">
-        <v>3.62</v>
-      </c>
-      <c r="G22" s="2">
-        <v>-3.18</v>
-      </c>
-      <c r="H22" s="2">
-        <v>4.3499999999999996</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>18</v>
-      </c>
-      <c r="B23" s="2">
-        <v>1.36</v>
-      </c>
-      <c r="C23" s="10">
-        <v>1</v>
-      </c>
-      <c r="D23" s="2">
-        <v>1.28</v>
-      </c>
-      <c r="E23" s="10">
-        <v>0</v>
-      </c>
-      <c r="F23" s="10">
-        <v>2</v>
-      </c>
-      <c r="G23" s="10">
-        <v>0</v>
-      </c>
-      <c r="H23" s="10">
-        <v>4</v>
-      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B24" s="2">
-        <v>55.1</v>
-      </c>
-      <c r="C24" s="2">
-        <v>54.5</v>
+        <v>0.25</v>
+      </c>
+      <c r="C24" s="8">
+        <v>-0.9</v>
       </c>
       <c r="D24" s="2">
-        <v>22.1</v>
-      </c>
-      <c r="E24" s="2">
-        <v>36.799999999999997</v>
+        <v>3.05</v>
+      </c>
+      <c r="E24" s="8">
+        <v>-3</v>
       </c>
       <c r="F24" s="2">
-        <v>72.5</v>
-      </c>
-      <c r="G24" s="11">
-        <v>20</v>
-      </c>
-      <c r="H24" s="11">
-        <v>94</v>
+        <v>3.62</v>
+      </c>
+      <c r="G24" s="2">
+        <v>-3.18</v>
+      </c>
+      <c r="H24" s="2">
+        <v>4.3499999999999996</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="11">
-        <v>29</v>
-      </c>
-      <c r="C25" s="2">
-        <v>27.4</v>
-      </c>
-      <c r="D25" s="11">
-        <v>9.98</v>
-      </c>
-      <c r="E25" s="2">
-        <v>22.9</v>
-      </c>
-      <c r="F25" s="2">
-        <v>31.4</v>
-      </c>
-      <c r="G25" s="2">
-        <v>17.7</v>
-      </c>
-      <c r="H25" s="2">
-        <v>71.7</v>
+        <v>18</v>
+      </c>
+      <c r="B25" s="2">
+        <v>1.36</v>
+      </c>
+      <c r="C25" s="8">
+        <v>1</v>
+      </c>
+      <c r="D25" s="2">
+        <v>1.28</v>
+      </c>
+      <c r="E25" s="8">
+        <v>0</v>
+      </c>
+      <c r="F25" s="8">
+        <v>2</v>
+      </c>
+      <c r="G25" s="8">
+        <v>0</v>
+      </c>
+      <c r="H25" s="8">
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="2">
+        <v>55.1</v>
+      </c>
+      <c r="C26" s="2">
+        <v>54.5</v>
+      </c>
+      <c r="D26" s="2">
+        <v>22.1</v>
+      </c>
+      <c r="E26" s="2">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="F26" s="2">
+        <v>72.5</v>
+      </c>
+      <c r="G26" s="9">
         <v>20</v>
       </c>
-      <c r="B26" s="2">
-        <v>1.5200000000000001E-4</v>
-      </c>
-      <c r="C26" s="2">
-        <v>1.4799999999999999E-4</v>
-      </c>
-      <c r="D26" s="2">
-        <v>3.4E-5</v>
-      </c>
-      <c r="E26" s="2">
-        <v>1.2400000000000001E-4</v>
-      </c>
-      <c r="F26" s="2">
-        <v>1.73E-4</v>
-      </c>
-      <c r="G26" s="2">
-        <v>9.8200000000000002E-5</v>
-      </c>
-      <c r="H26" s="2">
-        <v>2.32E-4</v>
+      <c r="H26" s="9">
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>21</v>
-      </c>
-      <c r="B27" s="2">
-        <v>3.0699999999999998E-3</v>
+        <v>23</v>
+      </c>
+      <c r="B27" s="9">
+        <v>29</v>
       </c>
       <c r="C27" s="2">
-        <v>3.0899999999999999E-3</v>
-      </c>
-      <c r="D27" s="2">
-        <v>8.4800000000000001E-4</v>
+        <v>27.4</v>
+      </c>
+      <c r="D27" s="9">
+        <v>9.98</v>
       </c>
       <c r="E27" s="2">
-        <v>2.7599999999999999E-3</v>
+        <v>22.9</v>
       </c>
       <c r="F27" s="2">
-        <v>3.1900000000000001E-3</v>
+        <v>31.4</v>
       </c>
       <c r="G27" s="2">
-        <v>6.4099999999999997E-4</v>
+        <v>17.7</v>
       </c>
       <c r="H27" s="2">
-        <v>6.94E-3</v>
+        <v>71.7</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="2">
+        <v>1.5200000000000001E-4</v>
+      </c>
+      <c r="C28" s="2">
+        <v>1.4799999999999999E-4</v>
+      </c>
+      <c r="D28" s="2">
+        <v>3.4E-5</v>
+      </c>
+      <c r="E28" s="2">
+        <v>1.2400000000000001E-4</v>
+      </c>
+      <c r="F28" s="2">
+        <v>1.73E-4</v>
+      </c>
+      <c r="G28" s="2">
+        <v>9.8200000000000002E-5</v>
+      </c>
+      <c r="H28" s="2">
+        <v>2.32E-4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>21</v>
+      </c>
+      <c r="B29" s="2">
+        <v>3.0699999999999998E-3</v>
+      </c>
+      <c r="C29" s="2">
+        <v>3.0899999999999999E-3</v>
+      </c>
+      <c r="D29" s="2">
+        <v>8.4800000000000001E-4</v>
+      </c>
+      <c r="E29" s="2">
+        <v>2.7599999999999999E-3</v>
+      </c>
+      <c r="F29" s="2">
+        <v>3.1900000000000001E-3</v>
+      </c>
+      <c r="G29" s="2">
+        <v>6.4099999999999997E-4</v>
+      </c>
+      <c r="H29" s="2">
+        <v>6.94E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
         <v>22</v>
       </c>
-      <c r="B28" s="11">
+      <c r="B30" s="9">
         <v>142</v>
       </c>
-      <c r="C28" s="11">
+      <c r="C30" s="9">
         <v>141</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D30" s="2">
         <v>15.9</v>
       </c>
-      <c r="E28" s="11">
+      <c r="E30" s="9">
         <v>132</v>
       </c>
-      <c r="F28" s="11">
+      <c r="F30" s="9">
         <v>151</v>
       </c>
-      <c r="G28" s="11">
+      <c r="G30" s="9">
         <v>102</v>
       </c>
-      <c r="H28" s="11">
+      <c r="H30" s="9">
         <v>177</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
     <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -1277,8 +1368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C94F0CD-7156-4A84-AB94-BC6F16265EF1}">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="73" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView zoomScale="73" workbookViewId="0">
+      <selection sqref="A1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1291,43 +1382,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="6"/>
-      <c r="B1" s="6"/>
-      <c r="C1" s="13" t="s">
+      <c r="A1" s="5"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="12" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="12"/>
+      <c r="B3" s="14"/>
       <c r="C3" s="2">
         <v>2361</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="7">
         <v>2327</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="7">
         <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B4" s="7"/>
+      <c r="B4" s="13"/>
       <c r="C4" s="2">
         <v>388</v>
       </c>
@@ -1339,7 +1430,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="8"/>
+      <c r="A5" s="6"/>
       <c r="B5" s="4"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -1474,10 +1565,10 @@
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="B16" s="3"/>
+      <c r="B16" s="11"/>
       <c r="C16" s="2">
         <v>2697</v>
       </c>
@@ -1489,10 +1580,10 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B17" s="3"/>
+      <c r="B17" s="11"/>
       <c r="C17" s="2">
         <v>52</v>
       </c>
@@ -1791,7 +1882,7 @@
       <c r="D40" s="2">
         <v>1067</v>
       </c>
-      <c r="E40" s="9">
+      <c r="E40" s="7">
         <v>9</v>
       </c>
     </row>
@@ -1922,4 +2013,379 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFAEE43F-AED4-467C-BF1A-314FED204738}">
+  <dimension ref="A1:F28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.453125" customWidth="1"/>
+    <col min="2" max="2" width="18.81640625" customWidth="1"/>
+    <col min="3" max="3" width="10.90625" customWidth="1"/>
+    <col min="4" max="4" width="16.6328125" customWidth="1"/>
+    <col min="5" max="5" width="14.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="5"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="12"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C2" s="12"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="14"/>
+      <c r="C3" s="3">
+        <v>2361</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="11"/>
+      <c r="F3" s="3">
+        <v>2697</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="13"/>
+      <c r="C4" s="3">
+        <v>388</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="11"/>
+      <c r="F4" s="3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="6"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="3">
+        <v>831</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="3"/>
+      <c r="B7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="3">
+        <v>246</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="3">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="3"/>
+      <c r="B8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1206</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="3">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="3"/>
+      <c r="B9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="3">
+        <v>466</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="3">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="3"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1483</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" t="s">
+        <v>45</v>
+      </c>
+      <c r="F11" s="3">
+        <v>1260</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="3"/>
+      <c r="B12" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1266</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" s="3">
+        <v>1489</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="3"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="3">
+        <v>584</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F14" s="3">
+        <v>1941</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="3"/>
+      <c r="B15" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="3">
+        <v>180</v>
+      </c>
+      <c r="E15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="3"/>
+      <c r="B16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="3">
+        <v>19</v>
+      </c>
+      <c r="E16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="3"/>
+      <c r="B17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" s="3">
+        <v>4</v>
+      </c>
+      <c r="E17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="3">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="3"/>
+      <c r="B18" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" s="3">
+        <v>403</v>
+      </c>
+      <c r="E18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="3">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="3"/>
+      <c r="B19" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="3">
+        <v>1559</v>
+      </c>
+      <c r="E19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" s="3">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C20" s="3"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="3">
+        <v>133</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E21" t="s">
+        <v>51</v>
+      </c>
+      <c r="F21" s="3">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="3"/>
+      <c r="B22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="3">
+        <v>1076</v>
+      </c>
+      <c r="E22" t="s">
+        <v>50</v>
+      </c>
+      <c r="F22" s="3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="3"/>
+      <c r="B23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="3">
+        <v>1510</v>
+      </c>
+      <c r="E23" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23" s="3">
+        <v>2471</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="3"/>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="3"/>
+      <c r="C25" s="3"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="3">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B27" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="3">
+        <v>2564</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C28" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
change the format of table
</commit_message>
<xml_diff>
--- a/summary_statistics.xlsx
+++ b/summary_statistics.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6940" activeTab="2" xr2:uid="{7B30B581-41F3-4625-9AEB-EDD9A381FEDF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6940" xr2:uid="{7B30B581-41F3-4625-9AEB-EDD9A381FEDF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -264,7 +264,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -272,11 +272,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -304,9 +313,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -317,6 +323,16 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -634,8 +650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B5EFC5A-2BC7-489C-88B9-EDFF87E125F6}">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView zoomScale="66" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" zoomScale="66" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -651,37 +667,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="2"/>
-      <c r="B1" s="10" t="s">
+      <c r="A1" s="14"/>
+      <c r="B1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="15" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
+      <c r="A2" s="16"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
@@ -1384,26 +1401,26 @@
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="14"/>
+      <c r="B3" s="13"/>
       <c r="C3" s="2">
         <v>2361</v>
       </c>
@@ -1415,10 +1432,10 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B4" s="13"/>
+      <c r="B4" s="12"/>
       <c r="C4" s="2">
         <v>388</v>
       </c>
@@ -1565,10 +1582,10 @@
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B16" s="11"/>
+      <c r="B16" s="10"/>
       <c r="C16" s="2">
         <v>2697</v>
       </c>
@@ -1580,10 +1597,10 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="B17" s="11"/>
+      <c r="B17" s="10"/>
       <c r="C17" s="2">
         <v>52</v>
       </c>
@@ -2019,7 +2036,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFAEE43F-AED4-467C-BF1A-314FED204738}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -2035,39 +2052,39 @@
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
       <c r="B1" s="5"/>
-      <c r="C1" s="12"/>
+      <c r="C1" s="11"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C2" s="12"/>
+      <c r="C2" s="11"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="B3" s="14"/>
+      <c r="B3" s="13"/>
       <c r="C3" s="3">
         <v>2361</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="11"/>
+      <c r="E3" s="10"/>
       <c r="F3" s="3">
         <v>2697</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B4" s="13"/>
+      <c r="B4" s="12"/>
       <c r="C4" s="3">
         <v>388</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="E4" s="11"/>
+      <c r="E4" s="10"/>
       <c r="F4" s="3">
         <v>52</v>
       </c>

</xml_diff>